<commit_message>
Updated programs version 2
</commit_message>
<xml_diff>
--- a/python/out.xlsx
+++ b/python/out.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>Student's names</t>
   </si>
@@ -31,25 +31,31 @@
     <t>Password</t>
   </si>
   <si>
-    <t>Chetan Kaushik</t>
+    <t>Contact No.</t>
+  </si>
+  <si>
+    <t>Fee status</t>
+  </si>
+  <si>
+    <t>Vaibhav Aggarwal</t>
   </si>
   <si>
     <t>Computer Engineering</t>
   </si>
   <si>
-    <t>chetan.kaushik.@computer.jcboseust.ac.in</t>
-  </si>
-  <si>
-    <t>*Y$Gk^7ZeK$</t>
-  </si>
-  <si>
-    <t>Dhruv Singh</t>
-  </si>
-  <si>
-    <t>dhruv.singh.@computer.jcboseust.ac.in</t>
-  </si>
-  <si>
-    <t>EI(*i?);$9Q</t>
+    <t>vaibhav.aggarwal.@computer.jcboseust.ac.in</t>
+  </si>
+  <si>
+    <t>&amp;negZrBrA8?</t>
+  </si>
+  <si>
+    <t>Vidushi Tickoo</t>
+  </si>
+  <si>
+    <t>vidushi.tickoo.@computer.jcboseust.ac.in</t>
+  </si>
+  <si>
+    <t>w:,^ROykm!|</t>
   </si>
 </sst>
 </file>
@@ -381,13 +387,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -403,39 +409,57 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>3001</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="F2">
+        <v>9764767579</v>
+      </c>
+      <c r="G2">
+        <v>45000</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>3002</v>
       </c>
       <c r="B3" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="E3" t="s">
-        <v>11</v>
+        <v>13</v>
+      </c>
+      <c r="F3">
+        <v>8920021900</v>
+      </c>
+      <c r="G3">
+        <v>45000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>